<commit_message>
Add remisiones & Update timbre examples
</commit_message>
<xml_diff>
--- a/documentos/images/DVZ_Tabla_PortalDesarr.xlsx
+++ b/documentos/images/DVZ_Tabla_PortalDesarr.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="43500" yWindow="1960" windowWidth="25520" windowHeight="23140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="docs" sheetId="1" r:id="rId1"/>
@@ -1038,10 +1038,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H41"/>
+  <dimension ref="B2:H42"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRuler="0" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:H35"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1052,73 +1052,52 @@
     <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="28">
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="18" t="s">
+    <row r="2" spans="2:8" ht="28">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G2" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="2:8" ht="15" customHeight="1">
-      <c r="B2" s="49" t="s">
+    <row r="3" spans="2:8" ht="15" customHeight="1">
+      <c r="B3" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="E2" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="G2" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8">
-      <c r="B3" s="45" t="s">
+      <c r="C3" s="50"/>
+      <c r="D3" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8">
+      <c r="B4" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="E3" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="F3" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="G3" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8">
-      <c r="B4" s="45"/>
-      <c r="C4" s="3" t="s">
-        <v>6</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>40</v>
@@ -1139,7 +1118,7 @@
     <row r="5" spans="2:8">
       <c r="B5" s="45"/>
       <c r="C5" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>40</v>
@@ -1160,7 +1139,7 @@
     <row r="6" spans="2:8">
       <c r="B6" s="45"/>
       <c r="C6" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>40</v>
@@ -1181,7 +1160,7 @@
     <row r="7" spans="2:8">
       <c r="B7" s="45"/>
       <c r="C7" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>40</v>
@@ -1202,7 +1181,7 @@
     <row r="8" spans="2:8">
       <c r="B8" s="45"/>
       <c r="C8" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>40</v>
@@ -1211,7 +1190,7 @@
         <v>40</v>
       </c>
       <c r="F8" s="22" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="G8" s="21" t="s">
         <v>40</v>
@@ -1223,7 +1202,7 @@
     <row r="9" spans="2:8">
       <c r="B9" s="45"/>
       <c r="C9" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>40</v>
@@ -1244,7 +1223,7 @@
     <row r="10" spans="2:8">
       <c r="B10" s="45"/>
       <c r="C10" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>40</v>
@@ -1253,7 +1232,7 @@
         <v>40</v>
       </c>
       <c r="F10" s="22" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="G10" s="21" t="s">
         <v>40</v>
@@ -1265,7 +1244,7 @@
     <row r="11" spans="2:8">
       <c r="B11" s="45"/>
       <c r="C11" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>40</v>
@@ -1286,7 +1265,7 @@
     <row r="12" spans="2:8">
       <c r="B12" s="45"/>
       <c r="C12" s="3" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>40</v>
@@ -1295,7 +1274,7 @@
         <v>40</v>
       </c>
       <c r="F12" s="22" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="G12" s="21" t="s">
         <v>40</v>
@@ -1307,7 +1286,7 @@
     <row r="13" spans="2:8">
       <c r="B13" s="45"/>
       <c r="C13" s="3" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="D13" s="12" t="s">
         <v>40</v>
@@ -1328,7 +1307,7 @@
     <row r="14" spans="2:8">
       <c r="B14" s="45"/>
       <c r="C14" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>40</v>
@@ -1349,7 +1328,7 @@
     <row r="15" spans="2:8">
       <c r="B15" s="45"/>
       <c r="C15" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>40</v>
@@ -1370,7 +1349,7 @@
     <row r="16" spans="2:8">
       <c r="B16" s="45"/>
       <c r="C16" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D16" s="12" t="s">
         <v>40</v>
@@ -1391,7 +1370,7 @@
     <row r="17" spans="2:8">
       <c r="B17" s="45"/>
       <c r="C17" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D17" s="12" t="s">
         <v>40</v>
@@ -1412,7 +1391,7 @@
     <row r="18" spans="2:8">
       <c r="B18" s="45"/>
       <c r="C18" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D18" s="12" t="s">
         <v>40</v>
@@ -1433,7 +1412,7 @@
     <row r="19" spans="2:8">
       <c r="B19" s="45"/>
       <c r="C19" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D19" s="12" t="s">
         <v>40</v>
@@ -1454,137 +1433,137 @@
     <row r="20" spans="2:8">
       <c r="B20" s="45"/>
       <c r="C20" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F20" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="G20" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8">
+      <c r="B21" s="45"/>
+      <c r="C21" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="E20" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="F20" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="G20" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8">
-      <c r="B21" s="43" t="s">
+      <c r="D21" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F21" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="G21" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8">
+      <c r="B22" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="E21" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="F21" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="G21" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="H21" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8">
-      <c r="B22" s="43"/>
-      <c r="C22" s="2" t="s">
+      <c r="D22" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="E22" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="F22" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="G22" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8">
+      <c r="B23" s="43"/>
+      <c r="C23" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="E22" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="F22" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="G22" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="H22" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8">
-      <c r="B23" s="44"/>
-      <c r="C23" s="8" t="s">
+      <c r="D23" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="F23" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="G23" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8">
+      <c r="B24" s="44"/>
+      <c r="C24" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D23" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="E23" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="F23" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="G23" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="H23" s="9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" ht="15" customHeight="1">
-      <c r="B24" s="49" t="s">
+      <c r="D24" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="F24" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="G24" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" ht="15" customHeight="1">
+      <c r="B25" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="C24" s="50"/>
-      <c r="D24" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E24" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="F24" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="G24" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="H24" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8">
-      <c r="B25" s="45" t="s">
+      <c r="C25" s="50"/>
+      <c r="D25" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="F25" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="G25" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8">
+      <c r="B26" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C26" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E25" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="F25" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="G25" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="H25" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8">
-      <c r="B26" s="45"/>
-      <c r="C26" s="3" t="s">
-        <v>30</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>48</v>
@@ -1605,7 +1584,7 @@
     <row r="27" spans="2:8">
       <c r="B27" s="45"/>
       <c r="C27" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>48</v>
@@ -1626,7 +1605,7 @@
     <row r="28" spans="2:8">
       <c r="B28" s="45"/>
       <c r="C28" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>48</v>
@@ -1647,7 +1626,7 @@
     <row r="29" spans="2:8">
       <c r="B29" s="45"/>
       <c r="C29" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>48</v>
@@ -1668,7 +1647,7 @@
     <row r="30" spans="2:8">
       <c r="B30" s="45"/>
       <c r="C30" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>48</v>
@@ -1689,7 +1668,7 @@
     <row r="31" spans="2:8">
       <c r="B31" s="45"/>
       <c r="C31" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D31" s="6" t="s">
         <v>48</v>
@@ -1710,7 +1689,7 @@
     <row r="32" spans="2:8">
       <c r="B32" s="45"/>
       <c r="C32" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D32" s="6" t="s">
         <v>48</v>
@@ -1731,7 +1710,7 @@
     <row r="33" spans="2:8">
       <c r="B33" s="45"/>
       <c r="C33" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>48</v>
@@ -1752,93 +1731,93 @@
     <row r="34" spans="2:8">
       <c r="B34" s="45"/>
       <c r="C34" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E34" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F34" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="G34" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8">
+      <c r="B35" s="45"/>
+      <c r="C35" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D34" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E34" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="F34" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="G34" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="H34" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="35" spans="2:8">
-      <c r="B35" s="46"/>
-      <c r="C35" s="10" t="s">
+      <c r="D35" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E35" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F35" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="G35" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8">
+      <c r="B36" s="46"/>
+      <c r="C36" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D35" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="E35" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="F35" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="G35" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="H35" s="11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="36" spans="2:8" ht="15" customHeight="1">
-      <c r="B36" s="49" t="s">
+      <c r="D36" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E36" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="F36" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="G36" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="H36" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" ht="15" customHeight="1">
+      <c r="B37" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="C36" s="50"/>
-      <c r="D36" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E36" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="F36" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="G36" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="H36" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="37" spans="2:8">
-      <c r="B37" s="47" t="s">
+      <c r="C37" s="50"/>
+      <c r="D37" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E37" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="F37" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="G37" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8">
+      <c r="B38" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C38" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E37" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="F37" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="G37" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="H37" s="12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="38" spans="2:8">
-      <c r="B38" s="47"/>
-      <c r="C38" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="D38" s="6" t="s">
         <v>48</v>
@@ -1859,7 +1838,7 @@
     <row r="39" spans="2:8">
       <c r="B39" s="47"/>
       <c r="C39" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D39" s="6" t="s">
         <v>48</v>
@@ -1880,54 +1859,75 @@
     <row r="40" spans="2:8">
       <c r="B40" s="47"/>
       <c r="C40" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E40" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F40" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="G40" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="H40" s="12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8">
+      <c r="B41" s="47"/>
+      <c r="C41" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D40" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E40" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="F40" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="G40" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="H40" s="13" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="41" spans="2:8">
-      <c r="B41" s="48"/>
-      <c r="C41" s="10" t="s">
+      <c r="D41" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E41" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="F41" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="G41" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="H41" s="13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8">
+      <c r="B42" s="48"/>
+      <c r="C42" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D41" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="E41" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="F41" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="G41" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="H41" s="14" t="s">
+      <c r="D42" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E42" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="F42" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="G42" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="H42" s="14" t="s">
         <v>48</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="B3:B20"/>
-    <mergeCell ref="B25:B35"/>
-    <mergeCell ref="B37:B41"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="B4:B21"/>
+    <mergeCell ref="B26:B36"/>
+    <mergeCell ref="B38:B42"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B37:C37"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -1942,7 +1942,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H5"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showGridLines="0" showRuler="0" workbookViewId="0">
       <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>

</xml_diff>